<commit_message>
Add more games. Add winners statistics in summarization excel
</commit_message>
<xml_diff>
--- a/analyze/data/2_bots_3_GPT/game1.xlsx
+++ b/analyze/data/2_bots_3_GPT/game1.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Narrations" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Votes" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Points" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Winners" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -9249,4 +9250,85 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Winner</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GPT Bot 3</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GPT Bot 1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bot 1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GPT Bot 2</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bot 2</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>